<commit_message>
updated excel data to have correct information and no duplicates
</commit_message>
<xml_diff>
--- a/data/excel/median_income_age.xlsx
+++ b/data/excel/median_income_age.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Texas A&amp;M\Senior\Fall 2021\CSCE 447 - Data Visualization\wage-gap\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Texas A&amp;M\Senior\Fall 2021\CSCE 447 - Data Visualization\wage-gap\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{140F0EA1-9A56-4FCD-8160-106C461811BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E987FC-F48A-4ECE-AB0A-6F91B8880715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="median_income_age" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -886,10 +886,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1212,876 +1214,6 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>24143</v>
-      </c>
-      <c r="B12">
-        <v>268</v>
-      </c>
-      <c r="C12">
-        <v>54024</v>
-      </c>
-      <c r="D12">
-        <v>156</v>
-      </c>
-      <c r="E12">
-        <v>60683</v>
-      </c>
-      <c r="F12">
-        <v>125</v>
-      </c>
-      <c r="G12">
-        <v>34381</v>
-      </c>
-      <c r="H12">
-        <v>97</v>
-      </c>
-      <c r="I12">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>23788</v>
-      </c>
-      <c r="B13">
-        <v>238</v>
-      </c>
-      <c r="C13">
-        <v>54768</v>
-      </c>
-      <c r="D13">
-        <v>207</v>
-      </c>
-      <c r="E13">
-        <v>61148</v>
-      </c>
-      <c r="F13">
-        <v>110</v>
-      </c>
-      <c r="G13">
-        <v>35107</v>
-      </c>
-      <c r="H13">
-        <v>120</v>
-      </c>
-      <c r="I13">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>24476</v>
-      </c>
-      <c r="B14">
-        <v>265</v>
-      </c>
-      <c r="C14">
-        <v>55821</v>
-      </c>
-      <c r="D14">
-        <v>143</v>
-      </c>
-      <c r="E14">
-        <v>62049</v>
-      </c>
-      <c r="F14">
-        <v>107</v>
-      </c>
-      <c r="G14">
-        <v>36743</v>
-      </c>
-      <c r="H14">
-        <v>108</v>
-      </c>
-      <c r="I14">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>25391</v>
-      </c>
-      <c r="B15">
-        <v>207</v>
-      </c>
-      <c r="C15">
-        <v>56987</v>
-      </c>
-      <c r="D15">
-        <v>164</v>
-      </c>
-      <c r="E15">
-        <v>63474</v>
-      </c>
-      <c r="F15">
-        <v>179</v>
-      </c>
-      <c r="G15">
-        <v>37847</v>
-      </c>
-      <c r="H15">
-        <v>137</v>
-      </c>
-      <c r="I15">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>27047</v>
-      </c>
-      <c r="B16">
-        <v>230</v>
-      </c>
-      <c r="C16">
-        <v>58970</v>
-      </c>
-      <c r="D16">
-        <v>223</v>
-      </c>
-      <c r="E16">
-        <v>65018</v>
-      </c>
-      <c r="F16">
-        <v>147</v>
-      </c>
-      <c r="G16">
-        <v>39186</v>
-      </c>
-      <c r="H16">
-        <v>107</v>
-      </c>
-      <c r="I16">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>28411</v>
-      </c>
-      <c r="B17">
-        <v>323</v>
-      </c>
-      <c r="C17">
-        <v>60810</v>
-      </c>
-      <c r="D17">
-        <v>107</v>
-      </c>
-      <c r="E17">
-        <v>67224</v>
-      </c>
-      <c r="F17">
-        <v>155</v>
-      </c>
-      <c r="G17">
-        <v>40971</v>
-      </c>
-      <c r="H17">
-        <v>123</v>
-      </c>
-      <c r="I17">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>30524</v>
-      </c>
-      <c r="B18">
-        <v>223</v>
-      </c>
-      <c r="C18">
-        <v>62815</v>
-      </c>
-      <c r="D18">
-        <v>204</v>
-      </c>
-      <c r="E18">
-        <v>69822</v>
-      </c>
-      <c r="F18">
-        <v>202</v>
-      </c>
-      <c r="G18">
-        <v>42113</v>
-      </c>
-      <c r="H18">
-        <v>138</v>
-      </c>
-      <c r="I18">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>120062818</v>
-      </c>
-      <c r="B19">
-        <v>161148</v>
-      </c>
-      <c r="C19">
-        <v>76</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>12</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>121520180</v>
-      </c>
-      <c r="B20">
-        <v>153217</v>
-      </c>
-      <c r="C20">
-        <v>76</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>12</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>122802852</v>
-      </c>
-      <c r="B21">
-        <v>137327</v>
-      </c>
-      <c r="C21">
-        <v>76</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>13</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>24143</v>
-      </c>
-      <c r="B22">
-        <v>268</v>
-      </c>
-      <c r="C22">
-        <v>54024</v>
-      </c>
-      <c r="D22">
-        <v>156</v>
-      </c>
-      <c r="E22">
-        <v>60683</v>
-      </c>
-      <c r="F22">
-        <v>125</v>
-      </c>
-      <c r="G22">
-        <v>34381</v>
-      </c>
-      <c r="H22">
-        <v>97</v>
-      </c>
-      <c r="I22">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>23788</v>
-      </c>
-      <c r="B23">
-        <v>238</v>
-      </c>
-      <c r="C23">
-        <v>54768</v>
-      </c>
-      <c r="D23">
-        <v>207</v>
-      </c>
-      <c r="E23">
-        <v>61148</v>
-      </c>
-      <c r="F23">
-        <v>110</v>
-      </c>
-      <c r="G23">
-        <v>35107</v>
-      </c>
-      <c r="H23">
-        <v>120</v>
-      </c>
-      <c r="I23">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>24476</v>
-      </c>
-      <c r="B24">
-        <v>265</v>
-      </c>
-      <c r="C24">
-        <v>55821</v>
-      </c>
-      <c r="D24">
-        <v>143</v>
-      </c>
-      <c r="E24">
-        <v>62049</v>
-      </c>
-      <c r="F24">
-        <v>107</v>
-      </c>
-      <c r="G24">
-        <v>36743</v>
-      </c>
-      <c r="H24">
-        <v>108</v>
-      </c>
-      <c r="I24">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>25391</v>
-      </c>
-      <c r="B25">
-        <v>207</v>
-      </c>
-      <c r="C25">
-        <v>56987</v>
-      </c>
-      <c r="D25">
-        <v>164</v>
-      </c>
-      <c r="E25">
-        <v>63474</v>
-      </c>
-      <c r="F25">
-        <v>179</v>
-      </c>
-      <c r="G25">
-        <v>37847</v>
-      </c>
-      <c r="H25">
-        <v>137</v>
-      </c>
-      <c r="I25">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>27047</v>
-      </c>
-      <c r="B26">
-        <v>230</v>
-      </c>
-      <c r="C26">
-        <v>58970</v>
-      </c>
-      <c r="D26">
-        <v>223</v>
-      </c>
-      <c r="E26">
-        <v>65018</v>
-      </c>
-      <c r="F26">
-        <v>147</v>
-      </c>
-      <c r="G26">
-        <v>39186</v>
-      </c>
-      <c r="H26">
-        <v>107</v>
-      </c>
-      <c r="I26">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>28411</v>
-      </c>
-      <c r="B27">
-        <v>323</v>
-      </c>
-      <c r="C27">
-        <v>60810</v>
-      </c>
-      <c r="D27">
-        <v>107</v>
-      </c>
-      <c r="E27">
-        <v>67224</v>
-      </c>
-      <c r="F27">
-        <v>155</v>
-      </c>
-      <c r="G27">
-        <v>40971</v>
-      </c>
-      <c r="H27">
-        <v>123</v>
-      </c>
-      <c r="I27">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>30524</v>
-      </c>
-      <c r="B28">
-        <v>223</v>
-      </c>
-      <c r="C28">
-        <v>62815</v>
-      </c>
-      <c r="D28">
-        <v>204</v>
-      </c>
-      <c r="E28">
-        <v>69822</v>
-      </c>
-      <c r="F28">
-        <v>202</v>
-      </c>
-      <c r="G28">
-        <v>42113</v>
-      </c>
-      <c r="H28">
-        <v>138</v>
-      </c>
-      <c r="I28">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>120062818</v>
-      </c>
-      <c r="B29">
-        <v>161148</v>
-      </c>
-      <c r="C29">
-        <v>76</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>12</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>121520180</v>
-      </c>
-      <c r="B30">
-        <v>153217</v>
-      </c>
-      <c r="C30">
-        <v>76</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>12</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <v>1</v>
-      </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-      <c r="I30">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>122802852</v>
-      </c>
-      <c r="B31">
-        <v>137327</v>
-      </c>
-      <c r="C31">
-        <v>76</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>13</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
-      <c r="I31">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>24143</v>
-      </c>
-      <c r="B32">
-        <v>268</v>
-      </c>
-      <c r="C32">
-        <v>54024</v>
-      </c>
-      <c r="D32">
-        <v>156</v>
-      </c>
-      <c r="E32">
-        <v>60683</v>
-      </c>
-      <c r="F32">
-        <v>125</v>
-      </c>
-      <c r="G32">
-        <v>34381</v>
-      </c>
-      <c r="H32">
-        <v>97</v>
-      </c>
-      <c r="I32">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>23788</v>
-      </c>
-      <c r="B33">
-        <v>238</v>
-      </c>
-      <c r="C33">
-        <v>54768</v>
-      </c>
-      <c r="D33">
-        <v>207</v>
-      </c>
-      <c r="E33">
-        <v>61148</v>
-      </c>
-      <c r="F33">
-        <v>110</v>
-      </c>
-      <c r="G33">
-        <v>35107</v>
-      </c>
-      <c r="H33">
-        <v>120</v>
-      </c>
-      <c r="I33">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>24476</v>
-      </c>
-      <c r="B34">
-        <v>265</v>
-      </c>
-      <c r="C34">
-        <v>55821</v>
-      </c>
-      <c r="D34">
-        <v>143</v>
-      </c>
-      <c r="E34">
-        <v>62049</v>
-      </c>
-      <c r="F34">
-        <v>107</v>
-      </c>
-      <c r="G34">
-        <v>36743</v>
-      </c>
-      <c r="H34">
-        <v>108</v>
-      </c>
-      <c r="I34">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>25391</v>
-      </c>
-      <c r="B35">
-        <v>207</v>
-      </c>
-      <c r="C35">
-        <v>56987</v>
-      </c>
-      <c r="D35">
-        <v>164</v>
-      </c>
-      <c r="E35">
-        <v>63474</v>
-      </c>
-      <c r="F35">
-        <v>179</v>
-      </c>
-      <c r="G35">
-        <v>37847</v>
-      </c>
-      <c r="H35">
-        <v>137</v>
-      </c>
-      <c r="I35">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>27047</v>
-      </c>
-      <c r="B36">
-        <v>230</v>
-      </c>
-      <c r="C36">
-        <v>58970</v>
-      </c>
-      <c r="D36">
-        <v>223</v>
-      </c>
-      <c r="E36">
-        <v>65018</v>
-      </c>
-      <c r="F36">
-        <v>147</v>
-      </c>
-      <c r="G36">
-        <v>39186</v>
-      </c>
-      <c r="H36">
-        <v>107</v>
-      </c>
-      <c r="I36">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>28411</v>
-      </c>
-      <c r="B37">
-        <v>323</v>
-      </c>
-      <c r="C37">
-        <v>60810</v>
-      </c>
-      <c r="D37">
-        <v>107</v>
-      </c>
-      <c r="E37">
-        <v>67224</v>
-      </c>
-      <c r="F37">
-        <v>155</v>
-      </c>
-      <c r="G37">
-        <v>40971</v>
-      </c>
-      <c r="H37">
-        <v>123</v>
-      </c>
-      <c r="I37">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>30524</v>
-      </c>
-      <c r="B38">
-        <v>223</v>
-      </c>
-      <c r="C38">
-        <v>62815</v>
-      </c>
-      <c r="D38">
-        <v>204</v>
-      </c>
-      <c r="E38">
-        <v>69822</v>
-      </c>
-      <c r="F38">
-        <v>202</v>
-      </c>
-      <c r="G38">
-        <v>42113</v>
-      </c>
-      <c r="H38">
-        <v>138</v>
-      </c>
-      <c r="I38">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>120062818</v>
-      </c>
-      <c r="B39">
-        <v>161148</v>
-      </c>
-      <c r="C39">
-        <v>76</v>
-      </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-      <c r="E39">
-        <v>12</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-      <c r="G39">
-        <v>1</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-      <c r="I39">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>121520180</v>
-      </c>
-      <c r="B40">
-        <v>153217</v>
-      </c>
-      <c r="C40">
-        <v>76</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40">
-        <v>12</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <v>1</v>
-      </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="I40">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>122802852</v>
-      </c>
-      <c r="B41">
-        <v>137327</v>
-      </c>
-      <c r="C41">
-        <v>76</v>
-      </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41">
-        <v>13</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41">
-        <v>2019</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>